<commit_message>
update import PURL IRI, import age from PATO using updated ontoFox input file, import age measurement datum manually by adding the terms in externalByhand.owl. The term will be imported using ontoDog when BFO2 based OBI is available
</commit_message>
<xml_diff>
--- a/ontology/external/ontoDog_input/ontoDog_input.xlsx
+++ b/ontology/external/ontoDog_input/ontoDog_input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="111">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t xml:space="preserve">http://purl.obolibrary.org/obo/IAO_0000231 </t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001167</t>
+  </si>
+  <si>
+    <t>age measurement datum</t>
   </si>
 </sst>
 </file>
@@ -696,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,7 +1255,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -1260,7 +1266,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -1271,7 +1277,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -1282,7 +1288,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -1293,7 +1299,21 @@
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" t="s">
+        <v>85</v>
+      </c>
+      <c r="E53" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added OBI terms from last release for OBIB
</commit_message>
<xml_diff>
--- a/ontology/external/ontoDog_input/ontoDog_input.xlsx
+++ b/ontology/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27226"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="21915" windowHeight="12015"/>
+    <workbookView xWindow="21020" yWindow="0" windowWidth="16800" windowHeight="20060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="207">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -349,6 +354,294 @@
   </si>
   <si>
     <t>age measurement datum</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001404</t>
+  </si>
+  <si>
+    <t>genetic characteristics information</t>
+  </si>
+  <si>
+    <t>containing a specimen function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002087 </t>
+  </si>
+  <si>
+    <t>specimen container</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002088 </t>
+  </si>
+  <si>
+    <t>physical store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002089 </t>
+  </si>
+  <si>
+    <t>specimen family creation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002095 </t>
+  </si>
+  <si>
+    <t>amniotic fluid specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002500 </t>
+  </si>
+  <si>
+    <t>bile specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002501 </t>
+  </si>
+  <si>
+    <t>cerebrospinal fluid specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002502 </t>
+  </si>
+  <si>
+    <t>feces specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002503 </t>
+  </si>
+  <si>
+    <t>digestive system fluid or secretion specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002504 </t>
+  </si>
+  <si>
+    <t>milk specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002505 </t>
+  </si>
+  <si>
+    <t>pericardial fluid specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002506 </t>
+  </si>
+  <si>
+    <t>saliva specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002507 </t>
+  </si>
+  <si>
+    <t>sputum specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002508 </t>
+  </si>
+  <si>
+    <t>sweat specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002509 </t>
+  </si>
+  <si>
+    <t>synovial fluid specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002510 </t>
+  </si>
+  <si>
+    <t>vitreous humor specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002511 </t>
+  </si>
+  <si>
+    <t>bone marrow specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002512 </t>
+  </si>
+  <si>
+    <t>placenta specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002513 </t>
+  </si>
+  <si>
+    <t>peritoneal fluid specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002514 </t>
+  </si>
+  <si>
+    <t>pleural fluid specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002515 </t>
+  </si>
+  <si>
+    <t>brain specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002516 </t>
+  </si>
+  <si>
+    <t>hair specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002517 </t>
+  </si>
+  <si>
+    <t>prostate gland specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002518 </t>
+  </si>
+  <si>
+    <t>skeletal muscle tissue specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002519 </t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI:0002520</t>
+  </si>
+  <si>
+    <t>heart specimen</t>
+  </si>
+  <si>
+    <t>renal medulla specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002521 </t>
+  </si>
+  <si>
+    <t>adrenal gland specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002522 </t>
+  </si>
+  <si>
+    <t>breast specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002523 </t>
+  </si>
+  <si>
+    <t>urinary bladder specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002524 </t>
+  </si>
+  <si>
+    <t>tibial artery specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002525 </t>
+  </si>
+  <si>
+    <t>skin of body specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002526 </t>
+  </si>
+  <si>
+    <t>pancreas specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002527 </t>
+  </si>
+  <si>
+    <t>stomach specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002528 </t>
+  </si>
+  <si>
+    <t>pituitary gland specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002529 </t>
+  </si>
+  <si>
+    <t>adipose tissue specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002530 </t>
+  </si>
+  <si>
+    <t>cortex of kidney specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002531 </t>
+  </si>
+  <si>
+    <t>esophagus mucosa specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002532 </t>
+  </si>
+  <si>
+    <t>colon specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002533 </t>
+  </si>
+  <si>
+    <t>lung specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002534 </t>
+  </si>
+  <si>
+    <t>esophagus muscularis mucosa specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002535 </t>
+  </si>
+  <si>
+    <t>cerebral cortex specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002536 </t>
+  </si>
+  <si>
+    <t>thyroid gland specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002537 </t>
+  </si>
+  <si>
+    <t>cerebellum specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002538 </t>
+  </si>
+  <si>
+    <t>tibial nerve specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002539 </t>
+  </si>
+  <si>
+    <t>coronary artery specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002540 </t>
+  </si>
+  <si>
+    <t>spleen specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002541 </t>
+  </si>
+  <si>
+    <t>aorta specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI:0002542 </t>
   </si>
 </sst>
 </file>
@@ -366,7 +659,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -393,14 +686,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -700,22 +990,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="57" customWidth="1"/>
-    <col min="2" max="2" width="49.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="49.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -732,7 +1022,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -743,7 +1033,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -754,7 +1044,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -765,7 +1055,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -776,7 +1066,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -787,7 +1077,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -798,7 +1088,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -809,7 +1099,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -820,7 +1110,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -831,7 +1121,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -842,7 +1132,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -856,7 +1146,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -867,7 +1157,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -878,7 +1168,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -889,7 +1179,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -900,7 +1190,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -911,7 +1201,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -922,7 +1212,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -933,7 +1223,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -944,7 +1234,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -955,7 +1245,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -966,7 +1256,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -977,7 +1267,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -988,7 +1278,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -999,7 +1289,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1010,7 +1300,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1021,7 +1311,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1032,7 +1322,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1043,7 +1333,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1054,7 +1344,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -1065,7 +1355,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1076,7 +1366,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1087,7 +1377,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1098,7 +1388,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1109,7 +1399,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -1120,7 +1410,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -1131,7 +1421,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -1142,7 +1432,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -1153,7 +1443,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -1164,7 +1454,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1175,7 +1465,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -1186,7 +1476,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -1200,7 +1490,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -1211,7 +1501,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -1222,7 +1512,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -1233,7 +1523,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -1244,7 +1534,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -1255,7 +1545,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -1266,7 +1556,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -1277,7 +1567,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -1288,7 +1578,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -1299,7 +1589,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -1313,14 +1603,545 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>128</v>
+      </c>
+      <c r="B62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>130</v>
+      </c>
+      <c r="B63" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" t="s">
+        <v>131</v>
+      </c>
+      <c r="C64" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65" t="s">
+        <v>133</v>
+      </c>
+      <c r="C65" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" t="s">
+        <v>135</v>
+      </c>
+      <c r="C66" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" t="s">
+        <v>137</v>
+      </c>
+      <c r="C67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>140</v>
+      </c>
+      <c r="B68" t="s">
+        <v>139</v>
+      </c>
+      <c r="C68" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>142</v>
+      </c>
+      <c r="B69" t="s">
+        <v>141</v>
+      </c>
+      <c r="C69" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>144</v>
+      </c>
+      <c r="B70" t="s">
+        <v>143</v>
+      </c>
+      <c r="C70" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>146</v>
+      </c>
+      <c r="B71" t="s">
+        <v>145</v>
+      </c>
+      <c r="C71" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72" t="s">
+        <v>147</v>
+      </c>
+      <c r="C72" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73" t="s">
+        <v>149</v>
+      </c>
+      <c r="C73" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>152</v>
+      </c>
+      <c r="B74" t="s">
+        <v>151</v>
+      </c>
+      <c r="C74" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>154</v>
+      </c>
+      <c r="B75" t="s">
+        <v>153</v>
+      </c>
+      <c r="C75" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>156</v>
+      </c>
+      <c r="B76" t="s">
+        <v>155</v>
+      </c>
+      <c r="C76" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>158</v>
+      </c>
+      <c r="B77" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>160</v>
+      </c>
+      <c r="B78" t="s">
+        <v>159</v>
+      </c>
+      <c r="C78" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>161</v>
+      </c>
+      <c r="B79" t="s">
+        <v>162</v>
+      </c>
+      <c r="C79" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>164</v>
+      </c>
+      <c r="B80" t="s">
+        <v>163</v>
+      </c>
+      <c r="C80" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>166</v>
+      </c>
+      <c r="B81" t="s">
+        <v>165</v>
+      </c>
+      <c r="C81" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" t="s">
+        <v>167</v>
+      </c>
+      <c r="C82" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>170</v>
+      </c>
+      <c r="B83" t="s">
+        <v>169</v>
+      </c>
+      <c r="C83" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>172</v>
+      </c>
+      <c r="B84" t="s">
+        <v>171</v>
+      </c>
+      <c r="C84" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>174</v>
+      </c>
+      <c r="B85" t="s">
+        <v>173</v>
+      </c>
+      <c r="C85" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>176</v>
+      </c>
+      <c r="B86" t="s">
+        <v>175</v>
+      </c>
+      <c r="C86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>178</v>
+      </c>
+      <c r="B87" t="s">
+        <v>177</v>
+      </c>
+      <c r="C87" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" t="s">
+        <v>179</v>
+      </c>
+      <c r="C88" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>182</v>
+      </c>
+      <c r="B89" t="s">
+        <v>181</v>
+      </c>
+      <c r="C89" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>184</v>
+      </c>
+      <c r="B90" t="s">
+        <v>183</v>
+      </c>
+      <c r="C90" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>186</v>
+      </c>
+      <c r="B91" t="s">
+        <v>185</v>
+      </c>
+      <c r="C91" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>188</v>
+      </c>
+      <c r="B92" t="s">
+        <v>187</v>
+      </c>
+      <c r="C92" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>190</v>
+      </c>
+      <c r="B93" t="s">
+        <v>189</v>
+      </c>
+      <c r="C93" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>192</v>
+      </c>
+      <c r="B94" t="s">
+        <v>191</v>
+      </c>
+      <c r="C94" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>194</v>
+      </c>
+      <c r="B95" t="s">
+        <v>193</v>
+      </c>
+      <c r="C95" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>196</v>
+      </c>
+      <c r="B96" t="s">
+        <v>195</v>
+      </c>
+      <c r="C96" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>198</v>
+      </c>
+      <c r="B97" t="s">
+        <v>197</v>
+      </c>
+      <c r="C97" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>200</v>
+      </c>
+      <c r="B98" t="s">
+        <v>199</v>
+      </c>
+      <c r="C98" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>202</v>
+      </c>
+      <c r="B99" t="s">
+        <v>201</v>
+      </c>
+      <c r="C99" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>204</v>
+      </c>
+      <c r="B100" t="s">
+        <v>203</v>
+      </c>
+      <c r="C100" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>206</v>
+      </c>
+      <c r="B101" t="s">
+        <v>205</v>
+      </c>
+      <c r="C101" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:E50">
     <sortCondition ref="B2:B50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1330,9 +2151,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1342,8 +2168,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added missing OBI terms and fixed survey data axiom
</commit_message>
<xml_diff>
--- a/ontology/external/ontoDog_input/ontoDog_input.xlsx
+++ b/ontology/external/ontoDog_input/ontoDog_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="3460" yWindow="3780" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="248">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -642,13 +642,136 @@
   </si>
   <si>
     <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002540 </t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GAZ_00000448</t>
+  </si>
+  <si>
+    <t>geographic location</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000029</t>
+  </si>
+  <si>
+    <t>numeral</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000100</t>
+  </si>
+  <si>
+    <t>data set</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000140</t>
+  </si>
+  <si>
+    <t>setting datum</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000300</t>
+  </si>
+  <si>
+    <t>textual entity</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000422</t>
+  </si>
+  <si>
+    <t>postal address</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000429</t>
+  </si>
+  <si>
+    <t>email address</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000577</t>
+  </si>
+  <si>
+    <t>CRID symbol</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000578</t>
+  </si>
+  <si>
+    <t>CRID</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000582</t>
+  </si>
+  <si>
+    <t>time stamped measurement datum</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000102</t>
+  </si>
+  <si>
+    <t>responsible party role</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000103</t>
+  </si>
+  <si>
+    <t>principal investigator role</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000274</t>
+  </si>
+  <si>
+    <t>adding a material entity into a target</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000444</t>
+  </si>
+  <si>
+    <t>target of material addition role</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001936</t>
+  </si>
+  <si>
+    <t>molecular-labeled material</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0302914</t>
+  </si>
+  <si>
+    <t>digital curation</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_1110087</t>
+  </si>
+  <si>
+    <t>donor role</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_1110109</t>
+  </si>
+  <si>
+    <t>target of material addition</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/REO_0000280</t>
+  </si>
+  <si>
+    <t>molecular label</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000408</t>
+  </si>
+  <si>
+    <t>length measurement datum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,6 +783,14 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -682,15 +813,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -990,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2129,6 +2264,226 @@
       </c>
       <c r="C101" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>207</v>
+      </c>
+      <c r="B102" t="s">
+        <v>208</v>
+      </c>
+      <c r="C102" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>210</v>
+      </c>
+      <c r="B103" t="s">
+        <v>211</v>
+      </c>
+      <c r="C103" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>212</v>
+      </c>
+      <c r="B104" t="s">
+        <v>213</v>
+      </c>
+      <c r="C104" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>214</v>
+      </c>
+      <c r="B105" t="s">
+        <v>215</v>
+      </c>
+      <c r="C105" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>216</v>
+      </c>
+      <c r="B106" t="s">
+        <v>217</v>
+      </c>
+      <c r="C106" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>246</v>
+      </c>
+      <c r="B107" t="s">
+        <v>247</v>
+      </c>
+      <c r="C107" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>218</v>
+      </c>
+      <c r="B108" t="s">
+        <v>219</v>
+      </c>
+      <c r="C108" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>220</v>
+      </c>
+      <c r="B109" t="s">
+        <v>221</v>
+      </c>
+      <c r="C109" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>222</v>
+      </c>
+      <c r="B110" t="s">
+        <v>223</v>
+      </c>
+      <c r="C110" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>224</v>
+      </c>
+      <c r="B111" t="s">
+        <v>225</v>
+      </c>
+      <c r="C111" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>226</v>
+      </c>
+      <c r="B112" t="s">
+        <v>227</v>
+      </c>
+      <c r="C112" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>228</v>
+      </c>
+      <c r="B113" t="s">
+        <v>229</v>
+      </c>
+      <c r="C113" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>230</v>
+      </c>
+      <c r="B114" t="s">
+        <v>231</v>
+      </c>
+      <c r="C114" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>232</v>
+      </c>
+      <c r="B115" t="s">
+        <v>233</v>
+      </c>
+      <c r="C115" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>234</v>
+      </c>
+      <c r="B116" t="s">
+        <v>235</v>
+      </c>
+      <c r="C116" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>236</v>
+      </c>
+      <c r="B117" t="s">
+        <v>237</v>
+      </c>
+      <c r="C117" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>238</v>
+      </c>
+      <c r="B118" t="s">
+        <v>239</v>
+      </c>
+      <c r="C118" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>240</v>
+      </c>
+      <c r="B119" t="s">
+        <v>241</v>
+      </c>
+      <c r="C119" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>242</v>
+      </c>
+      <c r="B120" t="s">
+        <v>243</v>
+      </c>
+      <c r="C120" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>244</v>
+      </c>
+      <c r="B121" t="s">
+        <v>245</v>
+      </c>
+      <c r="C121" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added obsolescence reason specification and instances
</commit_message>
<xml_diff>
--- a/ontology/external/ontoDog_input/ontoDog_input.xlsx
+++ b/ontology/external/ontoDog_input/ontoDog_input.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="250">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -765,6 +765,12 @@
   </si>
   <si>
     <t>length measurement datum</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000225</t>
+  </si>
+  <si>
+    <t>obsolescence reason specification</t>
   </si>
 </sst>
 </file>
@@ -1125,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2483,6 +2489,17 @@
         <v>245</v>
       </c>
       <c r="C121" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>248</v>
+      </c>
+      <c r="B122" t="s">
+        <v>249</v>
+      </c>
+      <c r="C122" t="s">
         <v>209</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added term replaced by annotation
</commit_message>
<xml_diff>
--- a/ontology/external/ontoDog_input/ontoDog_input.xlsx
+++ b/ontology/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="3460" yWindow="3780" windowWidth="25600" windowHeight="16060"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="252">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -771,6 +771,12 @@
   </si>
   <si>
     <t>obsolescence reason specification</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0100001</t>
+  </si>
+  <si>
+    <t>term replaced by</t>
   </si>
 </sst>
 </file>
@@ -1131,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="D124" sqref="D124"/>
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2500,6 +2506,17 @@
         <v>249</v>
       </c>
       <c r="C122" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
+        <v>250</v>
+      </c>
+      <c r="B123" t="s">
+        <v>251</v>
+      </c>
+      <c r="C123" t="s">
         <v>209</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add two terms in the file
</commit_message>
<xml_diff>
--- a/ontology/external/ontoDog_input/ontoDog_input.xlsx
+++ b/ontology/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27322"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="3780" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="3465" yWindow="3780" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="256">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -777,6 +777,18 @@
   </si>
   <si>
     <t>term replaced by</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000846</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001688</t>
+  </si>
+  <si>
+    <t>has organization member</t>
+  </si>
+  <si>
+    <t>is member of organization</t>
   </si>
 </sst>
 </file>
@@ -1137,22 +1149,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E123"/>
+  <dimension ref="A1:E125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57" customWidth="1"/>
-    <col min="2" max="2" width="49.1640625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1169,7 +1181,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1180,7 +1192,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1191,7 +1203,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1202,7 +1214,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1213,7 +1225,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1224,7 +1236,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1235,7 +1247,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1246,7 +1258,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1257,7 +1269,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1268,7 +1280,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1279,7 +1291,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -1293,7 +1305,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1304,7 +1316,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1315,7 +1327,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1326,7 +1338,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -1337,7 +1349,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1348,7 +1360,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1359,7 +1371,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1381,7 +1393,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1392,7 +1404,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1403,7 +1415,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -1414,7 +1426,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1425,7 +1437,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -1436,7 +1448,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1447,7 +1459,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1458,7 +1470,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1469,7 +1481,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1480,7 +1492,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1491,7 +1503,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -1502,7 +1514,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1513,7 +1525,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1524,7 +1536,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1535,7 +1547,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1546,7 +1558,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -1557,7 +1569,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -1568,7 +1580,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -1579,7 +1591,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -1590,7 +1602,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -1601,7 +1613,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1612,7 +1624,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -1623,7 +1635,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -1637,7 +1649,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -1648,7 +1660,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -1659,7 +1671,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -1670,7 +1682,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -1681,7 +1693,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -1692,7 +1704,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -1703,7 +1715,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -1714,7 +1726,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -1725,7 +1737,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -1736,7 +1748,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -1750,7 +1762,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -1761,7 +1773,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>160</v>
       </c>
@@ -1772,7 +1784,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>161</v>
       </c>
@@ -1783,7 +1795,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>162</v>
       </c>
@@ -1794,7 +1806,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -1805,7 +1817,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>164</v>
       </c>
@@ -1816,7 +1828,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>165</v>
       </c>
@@ -1827,7 +1839,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>166</v>
       </c>
@@ -1838,7 +1850,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>169</v>
       </c>
@@ -1849,7 +1861,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>170</v>
       </c>
@@ -1860,7 +1872,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>171</v>
       </c>
@@ -1871,7 +1883,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>172</v>
       </c>
@@ -1882,7 +1894,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>173</v>
       </c>
@@ -1893,7 +1905,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>174</v>
       </c>
@@ -1904,7 +1916,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>175</v>
       </c>
@@ -1915,7 +1927,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>176</v>
       </c>
@@ -1926,7 +1938,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -1937,7 +1949,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>178</v>
       </c>
@@ -1948,7 +1960,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>179</v>
       </c>
@@ -1959,7 +1971,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>180</v>
       </c>
@@ -1970,7 +1982,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>181</v>
       </c>
@@ -1981,7 +1993,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>182</v>
       </c>
@@ -1992,7 +2004,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>183</v>
       </c>
@@ -2003,7 +2015,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -2014,7 +2026,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>185</v>
       </c>
@@ -2025,7 +2037,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>186</v>
       </c>
@@ -2036,7 +2048,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>187</v>
       </c>
@@ -2047,7 +2059,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>188</v>
       </c>
@@ -2058,7 +2070,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>189</v>
       </c>
@@ -2069,7 +2081,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>190</v>
       </c>
@@ -2080,7 +2092,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>191</v>
       </c>
@@ -2091,7 +2103,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>192</v>
       </c>
@@ -2102,7 +2114,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>193</v>
       </c>
@@ -2113,7 +2125,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>194</v>
       </c>
@@ -2124,7 +2136,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>195</v>
       </c>
@@ -2135,7 +2147,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>196</v>
       </c>
@@ -2146,7 +2158,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>197</v>
       </c>
@@ -2157,7 +2169,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>198</v>
       </c>
@@ -2168,7 +2180,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>199</v>
       </c>
@@ -2179,7 +2191,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>200</v>
       </c>
@@ -2190,7 +2202,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>201</v>
       </c>
@@ -2201,7 +2213,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>202</v>
       </c>
@@ -2212,7 +2224,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>203</v>
       </c>
@@ -2223,7 +2235,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>204</v>
       </c>
@@ -2234,7 +2246,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>205</v>
       </c>
@@ -2245,7 +2257,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>206</v>
       </c>
@@ -2256,7 +2268,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>168</v>
       </c>
@@ -2267,7 +2279,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>167</v>
       </c>
@@ -2278,7 +2290,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>207</v>
       </c>
@@ -2289,7 +2301,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>210</v>
       </c>
@@ -2300,7 +2312,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>212</v>
       </c>
@@ -2311,7 +2323,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>214</v>
       </c>
@@ -2322,7 +2334,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>216</v>
       </c>
@@ -2333,7 +2345,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>246</v>
       </c>
@@ -2344,7 +2356,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>218</v>
       </c>
@@ -2355,7 +2367,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>220</v>
       </c>
@@ -2366,7 +2378,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>222</v>
       </c>
@@ -2377,7 +2389,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>224</v>
       </c>
@@ -2388,7 +2400,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>226</v>
       </c>
@@ -2399,7 +2411,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>228</v>
       </c>
@@ -2410,7 +2422,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>230</v>
       </c>
@@ -2421,7 +2433,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>232</v>
       </c>
@@ -2432,7 +2444,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>234</v>
       </c>
@@ -2443,7 +2455,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>236</v>
       </c>
@@ -2454,7 +2466,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>238</v>
       </c>
@@ -2465,7 +2477,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>240</v>
       </c>
@@ -2476,7 +2488,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>242</v>
       </c>
@@ -2487,7 +2499,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -2498,7 +2510,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>248</v>
       </c>
@@ -2509,7 +2521,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>250</v>
       </c>
@@ -2518,6 +2530,28 @@
       </c>
       <c r="C123" t="s">
         <v>209</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>252</v>
+      </c>
+      <c r="B124" t="s">
+        <v>255</v>
+      </c>
+      <c r="C124" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>253</v>
+      </c>
+      <c r="B125" t="s">
+        <v>254</v>
+      </c>
+      <c r="C125" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2540,7 +2574,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2557,7 +2591,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>